<commit_message>
SMType download and Create page implemented SOCode insertion into Tbl_Mst_SalesmanRouteMapping
</commit_message>
<xml_diff>
--- a/Excel/SampleSSMType.xlsx
+++ b/Excel/SampleSSMType.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g116036\source\repos\Route\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9619BFEC-765F-4170-8D75-49A6244863CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10653450-68CC-4FC3-BAD3-DC5566B981EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0101E622-CFF6-4BF4-B31A-A5CE0D81BBBA}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SSMType</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>SYNAPSE</t>
+  </si>
+  <si>
+    <t>SMCode</t>
   </si>
 </sst>
 </file>
@@ -441,15 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AD1F16-3DE6-4596-849C-231D277E0340}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,6 +482,9 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>